<commit_message>
Deleted Excel Files, modified xml
</commit_message>
<xml_diff>
--- a/src/test/resources/TestScript.xlsx
+++ b/src/test/resources/TestScript.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\eclipse-workspace\Vtiger_Project\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98B174B3-3188-4A96-BB18-A2F291AB7E4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8F29F0-7003-476F-B816-C048B42A970E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" r:id="rId1"/>
+    <sheet name="Organization" sheetId="2" r:id="rId2"/>
+    <sheet name="Contact" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>ProductName</t>
   </si>
@@ -40,6 +42,36 @@
   </si>
   <si>
     <t>CIA_</t>
+  </si>
+  <si>
+    <t>OrgName</t>
+  </si>
+  <si>
+    <t>ISIS_</t>
+  </si>
+  <si>
+    <t>Mujhahideen_</t>
+  </si>
+  <si>
+    <t>hamas_</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>sunil</t>
+  </si>
+  <si>
+    <t>samal</t>
+  </si>
+  <si>
+    <t>raju</t>
+  </si>
+  <si>
+    <t>khanna</t>
   </si>
 </sst>
 </file>
@@ -81,7 +113,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -101,6 +144,27 @@
     <tableColumn id="1" xr3:uid="{4629FD69-4073-49A5-82D8-FB369C8268D4}" name="ProductName"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{21537370-D90C-4020-884D-0EE1F8A4904A}" name="Table1" displayName="Table1" ref="A1:A4" totalsRowShown="0">
+  <autoFilter ref="A1:A4" xr:uid="{21537370-D90C-4020-884D-0EE1F8A4904A}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{F59F7FD4-6C21-494B-BF44-90D7DC548B6C}" name="OrgName"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0562F476-35A1-4102-8365-60DAEAAD1438}" name="Table14" displayName="Table14" ref="A1:B3" totalsRowShown="0">
+  <autoFilter ref="A1:B3" xr:uid="{0562F476-35A1-4102-8365-60DAEAAD1438}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{0DB1C7E8-C5F0-43F1-B302-5839EB072218}" name="FirstName"/>
+    <tableColumn id="2" xr3:uid="{B7B2507B-D47C-4800-893A-2204FC2B07AB}" name="LastName"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -369,7 +433,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -411,4 +475,96 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758EB333-3943-4CED-AE57-97EF065DCC63}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A2:A4">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="ISIS_">
+      <formula>NOT(ISERROR(SEARCH("ISIS_",A2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1882D86-9B54-4E7C-B2B7-D50BFD2F9D78}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+    <col min="2" max="2" width="17.453125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Refactor framework: add XlUtility and DataProvider, update Product & Org tests
- Added `XlUtility` for centralized Excel read/write operations
- Added `dataProvider` package for module-wise test data (Product, Organization, Opportunity)
- Updated `ProductFlowTest` and `OrgFlowTest` to use DataProvider for data-driven testing
- Modified `BaseClass` and `configUtility` to support framework improvements
- Updated `OpportunitiesPage` for page enhancements
- Updated `TestScript.xlsx` with test data for new DataProviders
- TestNG reports updated (test-output folder)
</commit_message>
<xml_diff>
--- a/src/test/resources/TestScript.xlsx
+++ b/src/test/resources/TestScript.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\eclipse-workspace\Vtiger_Project\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8F29F0-7003-476F-B816-C048B42A970E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F4A9C6-D019-4B3E-846F-43BFF491F623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" r:id="rId1"/>
     <sheet name="Organization" sheetId="2" r:id="rId2"/>
-    <sheet name="Contact" sheetId="3" r:id="rId3"/>
+    <sheet name="Opportunities" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,51 +27,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>ProductName</t>
   </si>
   <si>
-    <t>QSP_</t>
-  </si>
-  <si>
-    <t>ISI_</t>
-  </si>
-  <si>
     <t>RAW_</t>
   </si>
   <si>
-    <t>CIA_</t>
-  </si>
-  <si>
     <t>OrgName</t>
   </si>
   <si>
-    <t>ISIS_</t>
-  </si>
-  <si>
-    <t>Mujhahideen_</t>
-  </si>
-  <si>
     <t>hamas_</t>
   </si>
   <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
-  <si>
-    <t>sunil</t>
-  </si>
-  <si>
-    <t>samal</t>
-  </si>
-  <si>
-    <t>raju</t>
-  </si>
-  <si>
-    <t>khanna</t>
+    <t>Opportunity Name</t>
+  </si>
+  <si>
+    <t>AsiaCup</t>
+  </si>
+  <si>
+    <t>ExpectedError</t>
   </si>
 </sst>
 </file>
@@ -138,18 +114,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B3A8396A-EF2B-4CF2-A8DB-ABF6862FA743}" name="Table2" displayName="Table2" ref="A1:A5" totalsRowShown="0">
-  <autoFilter ref="A1:A5" xr:uid="{B3A8396A-EF2B-4CF2-A8DB-ABF6862FA743}"/>
-  <tableColumns count="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B3A8396A-EF2B-4CF2-A8DB-ABF6862FA743}" name="Table2" displayName="Table2" ref="A1:B2" totalsRowShown="0">
+  <autoFilter ref="A1:B2" xr:uid="{B3A8396A-EF2B-4CF2-A8DB-ABF6862FA743}"/>
+  <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{4629FD69-4073-49A5-82D8-FB369C8268D4}" name="ProductName"/>
+    <tableColumn id="2" xr3:uid="{52574D1B-591D-4F1F-93EC-61E1FE9142C4}" name="ExpectedError"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{21537370-D90C-4020-884D-0EE1F8A4904A}" name="Table1" displayName="Table1" ref="A1:A4" totalsRowShown="0">
-  <autoFilter ref="A1:A4" xr:uid="{21537370-D90C-4020-884D-0EE1F8A4904A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{21537370-D90C-4020-884D-0EE1F8A4904A}" name="Table1" displayName="Table1" ref="A1:A2" totalsRowShown="0">
+  <autoFilter ref="A1:A2" xr:uid="{21537370-D90C-4020-884D-0EE1F8A4904A}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{F59F7FD4-6C21-494B-BF44-90D7DC548B6C}" name="OrgName"/>
   </tableColumns>
@@ -158,11 +135,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0562F476-35A1-4102-8365-60DAEAAD1438}" name="Table14" displayName="Table14" ref="A1:B3" totalsRowShown="0">
-  <autoFilter ref="A1:B3" xr:uid="{0562F476-35A1-4102-8365-60DAEAAD1438}"/>
-  <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{0DB1C7E8-C5F0-43F1-B302-5839EB072218}" name="FirstName"/>
-    <tableColumn id="2" xr3:uid="{B7B2507B-D47C-4800-893A-2204FC2B07AB}" name="LastName"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0562F476-35A1-4102-8365-60DAEAAD1438}" name="Table14" displayName="Table14" ref="A1:A3" totalsRowShown="0">
+  <autoFilter ref="A1:A3" xr:uid="{0562F476-35A1-4102-8365-60DAEAAD1438}"/>
+  <tableColumns count="1">
+    <tableColumn id="1" xr3:uid="{0DB1C7E8-C5F0-43F1-B302-5839EB072218}" name="Opportunity Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -431,10 +407,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -444,29 +420,17 @@
     <col min="3" max="3" width="17.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -479,10 +443,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758EB333-3943-4CED-AE57-97EF065DCC63}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -492,26 +456,16 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A4">
+  <conditionalFormatting sqref="A2">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="ISIS_">
       <formula>NOT(ISERROR(SEARCH("ISIS_",A2)))</formula>
     </cfRule>
@@ -525,10 +479,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1882D86-9B54-4E7C-B2B7-D50BFD2F9D78}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -537,28 +491,14 @@
     <col min="2" max="2" width="17.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: Integrate Organisation-Opportunity flow and Excel data handling
- Updated OpportunitiesPage to handle popup window for selecting Organisation
- Added setCellData method in XlUtility for storing dynamic Org names
- Modified OrgFlowTest to save created Organisation name into Excel
- Updated OpportunitiesFlowTest to fetch Org name from Excel and link it to Opportunities
- Adjusted OpportunityDataProvider and ProductFlowTest for improved data handling
- Updated TestScript.xlsx with OrgData sheet for storing dynamic organisation names
</commit_message>
<xml_diff>
--- a/src/test/resources/TestScript.xlsx
+++ b/src/test/resources/TestScript.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\eclipse-workspace\Vtiger_Project\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F4A9C6-D019-4B3E-846F-43BFF491F623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E24A2FD-F09C-4FAB-A6BB-D8B3A94F46A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product" sheetId="1" r:id="rId1"/>
     <sheet name="Organization" sheetId="2" r:id="rId2"/>
     <sheet name="Opportunities" sheetId="3" r:id="rId3"/>
+    <sheet name="OrgData" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>ProductName</t>
   </si>
@@ -71,7 +72,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -79,12 +80,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -445,8 +462,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758EB333-3943-4CED-AE57-97EF065DCC63}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -482,7 +499,7 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -507,4 +524,30 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A28B5AE1-1561-41C4-A627-CE3694F26AC5}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="16.81640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
git commit -m "Fix Opportunity creation flow: updated OpportunitiesPage POM, test data handling, and Excel utility for org linkage"
</commit_message>
<xml_diff>
--- a/src/test/resources/TestScript.xlsx
+++ b/src/test/resources/TestScript.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\eclipse-workspace\Vtiger_Project\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E24A2FD-F09C-4FAB-A6BB-D8B3A94F46A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59F86017-EEF3-4388-AE8A-692C70E5A3E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>ProductName</t>
   </si>
@@ -49,12 +49,16 @@
   </si>
   <si>
     <t>ExpectedError</t>
+  </si>
+  <si>
+    <t>hamas_258</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -432,21 +436,21 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.26953125" customWidth="1"/>
-    <col min="2" max="2" width="14.453125" customWidth="1"/>
-    <col min="3" max="3" width="17.36328125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="15.26953125"/>
+    <col min="2" max="2" customWidth="true" width="14.453125"/>
+    <col min="3" max="3" customWidth="true" width="17.36328125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" t="s" s="0">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>1</v>
       </c>
     </row>
@@ -468,16 +472,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.81640625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="15.81640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>3</v>
       </c>
     </row>
@@ -504,17 +508,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.81640625" customWidth="1"/>
-    <col min="2" max="2" width="17.453125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="15.81640625"/>
+    <col min="2" max="2" customWidth="true" width="17.453125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" t="s" s="0">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>5</v>
       </c>
     </row>
@@ -531,12 +535,12 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.81640625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="16.81640625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
@@ -545,7 +549,9 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>